<commit_message>
added rows will have orange backgrouds in the Excel table
</commit_message>
<xml_diff>
--- a/output/parametres_mis_a_jour.xlsx
+++ b/output/parametres_mis_a_jour.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univbourgogne-my.sharepoint.com/personal/hatim_bahand_etu_ube_fr/Documents/Bureau/contract_synthesizer/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_45FB4BCFBD61B8CD1A947FF1ABA649A0E910D142" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1507FEE0-EAE1-4313-8BB3-D59106F76C0C}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_4513F020BB564C5D16C78F3F51C279F7D4687970" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14328ABA-4B12-4DD3-AAB3-9412AFCF99A5}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2628" yWindow="1908" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2628" yWindow="1908" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
handle the changes in the table cell by cell
</commit_message>
<xml_diff>
--- a/output/parametres_mis_a_jour.xlsx
+++ b/output/parametres_mis_a_jour.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univbourgogne-my.sharepoint.com/personal/hatim_bahand_etu_ube_fr/Documents/Bureau/contract_synthesizer/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_4513F020BB564C5D16C78F3F51C279F7D4687970" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14328ABA-4B12-4DD3-AAB3-9412AFCF99A5}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_A3D15F591C9F58B9CC02FD60DAAE2ABA881758FF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B06260D-E84C-4478-93F8-6BEC1030FFFE}"/>
   <bookViews>
     <workbookView xWindow="2628" yWindow="1908" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,7 +492,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding a python simple GUI
</commit_message>
<xml_diff>
--- a/output/parametres_mis_a_jour.xlsx
+++ b/output/parametres_mis_a_jour.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univbourgogne-my.sharepoint.com/personal/hatim_bahand_etu_ube_fr/Documents/Bureau/contract_synthesizer/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_A3D15F591C9F58B9CC02FD60DAAE2ABA881758FF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B06260D-E84C-4478-93F8-6BEC1030FFFE}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_CBF90CD39D90A8E9CC5D79A3E3E82D3C289C221A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{638F509B-9597-4806-992E-938D8BC881B8}"/>
   <bookViews>
-    <workbookView xWindow="2628" yWindow="1908" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>

</xml_diff>